<commit_message>
Revert from umap-dbscan to kmeans, reassign strategies and categories, switch from clusters to categories, make a dendrogram of categories with strategies and a map of localmoran i, make other changes, delete useless code from script, #4
</commit_message>
<xml_diff>
--- a/law-firms-names/journal-article/cluster-labels.xlsx
+++ b/law-firms-names/journal-article/cluster-labels.xlsx
@@ -8,8 +8,11 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="cluster-labels" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="cluster-labels" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'cluster-labels'!$A$1:$H$51</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="118">
   <si>
     <t xml:space="preserve">cluster</t>
   </si>
@@ -37,6 +40,9 @@
     <t xml:space="preserve">group</t>
   </si>
   <si>
+    <t xml:space="preserve">category</t>
+  </si>
+  <si>
     <t xml:space="preserve">strategy</t>
   </si>
   <si>
@@ -52,7 +58,7 @@
     <t xml:space="preserve">Law</t>
   </si>
   <si>
-    <t xml:space="preserve">B</t>
+    <t xml:space="preserve">Belonging</t>
   </si>
   <si>
     <t xml:space="preserve">Includes names with one of three Russian words: “эксперт” (expert), “советник“ (advisor), “консультант” (consultant)</t>
@@ -67,7 +73,10 @@
     <t xml:space="preserve">Service</t>
   </si>
   <si>
-    <t xml:space="preserve">BM</t>
+    <t xml:space="preserve">Expert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Market</t>
   </si>
   <si>
     <t xml:space="preserve">Names including the word “компания” (company) or other similar words (“фирма“ — firm, “корпорация” — corporation)</t>
@@ -82,13 +91,16 @@
     <t xml:space="preserve">Form</t>
   </si>
   <si>
+    <t xml:space="preserve">Law firm</t>
+  </si>
+  <si>
     <t xml:space="preserve">A mixture of short names without apparent regularities</t>
   </si>
   <si>
     <t xml:space="preserve">Misc</t>
   </si>
   <si>
-    <t xml:space="preserve">N</t>
+    <t xml:space="preserve">No-strategy</t>
   </si>
   <si>
     <t xml:space="preserve">A mixture of names that include a subword “юр” (first letters of the Russian word meaning “juridical”) or start with the letter “ю” (probably meaning the same “juridical”)</t>
@@ -136,7 +148,10 @@
     <t xml:space="preserve">Finance</t>
   </si>
   <si>
-    <t xml:space="preserve">M</t>
+    <t xml:space="preserve">Audit&amp;Finance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uniqueness</t>
   </si>
   <si>
     <t xml:space="preserve">Names containing the word “партнёрство” (partnership) or other words meaning some kind of union: “группа компаний” (group of companies), “альянс” (alliance)</t>
@@ -145,6 +160,9 @@
     <t xml:space="preserve">Partnership, Alliance</t>
   </si>
   <si>
+    <t xml:space="preserve">Parthership</t>
+  </si>
+  <si>
     <t xml:space="preserve">A mixture of names without apparent regularities, except for the Cyrillic letter “в” present in the majority of them</t>
   </si>
   <si>
@@ -157,6 +175,9 @@
     <t xml:space="preserve">Protection</t>
   </si>
   <si>
+    <t xml:space="preserve">Legal aid</t>
+  </si>
+  <si>
     <t xml:space="preserve">A mixture of names without apparent regularities, except for the Cyrillic letter “к” present in the majority of them</t>
   </si>
   <si>
@@ -166,6 +187,9 @@
     <t xml:space="preserve">Real estate</t>
   </si>
   <si>
+    <t xml:space="preserve">Property&amp;Development</t>
+  </si>
+  <si>
     <t xml:space="preserve">Names pointing to a construction industry with the words “строй“ (build), “проект” (project), “девелоп” (develop)</t>
   </si>
   <si>
@@ -211,7 +235,7 @@
     <t xml:space="preserve">Partners</t>
   </si>
   <si>
-    <t xml:space="preserve">U</t>
+    <t xml:space="preserve">Personal brand</t>
   </si>
   <si>
     <t xml:space="preserve">Names following the pattern “juridical/legal company/firm/bureau/agency person name(s) + partners”</t>
@@ -220,9 +244,6 @@
     <t xml:space="preserve">Juridical, Legal, Company, Firm, Bureau, Partners</t>
   </si>
   <si>
-    <t xml:space="preserve">BU</t>
-  </si>
-  <si>
     <t xml:space="preserve">Names following the pattern “jurudical/legal company/firm/alliance”</t>
   </si>
   <si>
@@ -244,6 +265,9 @@
     <t xml:space="preserve">Technology</t>
   </si>
   <si>
+    <t xml:space="preserve">EdSciTech</t>
+  </si>
+  <si>
     <t xml:space="preserve">Names typically with the words ”управляющая компания” (managing company) or similar; probably the majority of these names is related to housing services that are provided by ”house managing companies” in Russia, but sometimes are likely to relate to business and investment</t>
   </si>
   <si>
@@ -253,6 +277,9 @@
     <t xml:space="preserve">Management</t>
   </si>
   <si>
+    <t xml:space="preserve">Managing companies</t>
+  </si>
+  <si>
     <t xml:space="preserve">Names with the word “плюс” (plus) or a plus (+) symbol</t>
   </si>
   <si>
@@ -265,6 +292,9 @@
     <t xml:space="preserve">Garant</t>
   </si>
   <si>
+    <t xml:space="preserve">Guarantor</t>
+  </si>
+  <si>
     <t xml:space="preserve">Names with the word “центр” (center), usually “юридический” (juridical)</t>
   </si>
   <si>
@@ -319,10 +349,16 @@
     <t xml:space="preserve">Legal, Juridical, Service</t>
   </si>
   <si>
+    <t xml:space="preserve">Legal service</t>
+  </si>
+  <si>
     <t xml:space="preserve">Various names, some of them have positive legal-related connotations, such as “дела в порядке” (everything is right), “норма” (norm)</t>
   </si>
   <si>
     <t xml:space="preserve">Misc, Positive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Positive</t>
   </si>
   <si>
     <t xml:space="preserve">Names about support and help (“защита” — protection, “поддержка” — support). Tend to be less securitized than in cluster #14. Usually include the word “центр” (center)</t>
@@ -350,7 +386,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -384,6 +420,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -428,25 +469,29 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -458,77 +503,202 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F43" activeCellId="0" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="72.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="25.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="19.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="72.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.94"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="14.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.94"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.54"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row r="1" s="2" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -536,22 +706,25 @@
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="D3" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -559,22 +732,25 @@
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="C4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -582,22 +758,25 @@
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>21</v>
+      <c r="B5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -605,22 +784,25 @@
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>9</v>
+      <c r="B6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="1" t="n">
+      <c r="G6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -628,22 +810,25 @@
       <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>21</v>
+      <c r="B7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -651,22 +836,25 @@
       <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>21</v>
+      <c r="B8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -674,22 +862,25 @@
       <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>31</v>
+      <c r="B9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -697,22 +888,25 @@
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>9</v>
+      <c r="B10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="1" t="n">
+      <c r="G10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -720,22 +914,25 @@
       <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>21</v>
+      <c r="B11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -743,22 +940,25 @@
       <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>37</v>
+      <c r="B12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -766,22 +966,25 @@
       <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>18</v>
+      <c r="B13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -789,22 +992,25 @@
       <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>21</v>
+      <c r="B14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -812,22 +1018,25 @@
       <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>44</v>
+      <c r="B15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -835,22 +1044,25 @@
       <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>21</v>
+      <c r="B16" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -858,22 +1070,25 @@
       <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>47</v>
+      <c r="B17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G17" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -881,22 +1096,25 @@
       <c r="A18" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>47</v>
+      <c r="B18" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H18" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -904,22 +1122,25 @@
       <c r="A19" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>21</v>
+      <c r="B19" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G19" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -927,22 +1148,25 @@
       <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>31</v>
+      <c r="B20" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -950,22 +1174,25 @@
       <c r="A21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>21</v>
+      <c r="B21" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G21" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -973,22 +1200,25 @@
       <c r="A22" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>21</v>
+      <c r="B22" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G22" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -996,22 +1226,25 @@
       <c r="A23" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>13</v>
+      <c r="B23" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G23" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1019,22 +1252,25 @@
       <c r="A24" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>13</v>
+      <c r="B24" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G24" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H24" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1042,22 +1278,25 @@
       <c r="A25" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>14</v>
+      <c r="B25" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G25" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1065,22 +1304,25 @@
       <c r="A26" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>31</v>
+      <c r="B26" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G26" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1088,22 +1330,25 @@
       <c r="A27" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>9</v>
+      <c r="B27" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G27" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1111,22 +1356,25 @@
       <c r="A28" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>18</v>
+      <c r="B28" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G28" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1134,22 +1382,25 @@
       <c r="A29" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>21</v>
+      <c r="B29" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G29" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H29" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1157,22 +1408,25 @@
       <c r="A30" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>21</v>
+      <c r="B30" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G30" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H30" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1180,22 +1434,25 @@
       <c r="A31" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>31</v>
+      <c r="B31" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G31" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1203,22 +1460,25 @@
       <c r="A32" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>31</v>
+      <c r="B32" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G32" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1226,22 +1486,25 @@
       <c r="A33" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>37</v>
+      <c r="B33" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G33" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H33" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1249,22 +1512,25 @@
       <c r="A34" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>21</v>
+      <c r="B34" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G34" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H34" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1272,22 +1538,25 @@
       <c r="A35" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>73</v>
+      <c r="B35" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G35" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H35" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1295,22 +1564,25 @@
       <c r="A36" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>76</v>
+      <c r="B36" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G36" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H36" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1318,22 +1590,25 @@
       <c r="A37" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>21</v>
+      <c r="B37" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G37" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H37" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1341,22 +1616,25 @@
       <c r="A38" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>44</v>
+      <c r="B38" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G38" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H38" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1364,22 +1642,25 @@
       <c r="A39" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>31</v>
+      <c r="B39" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G39" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1387,22 +1668,25 @@
       <c r="A40" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>21</v>
+      <c r="B40" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G40" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H40" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1410,22 +1694,25 @@
       <c r="A41" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>21</v>
+      <c r="B41" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G41" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H41" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1433,22 +1720,25 @@
       <c r="A42" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>18</v>
+      <c r="B42" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G42" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H42" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1456,22 +1746,25 @@
       <c r="A43" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>90</v>
+      <c r="B43" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>99</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G43" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H43" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1479,22 +1772,25 @@
       <c r="A44" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>37</v>
+      <c r="B44" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G44" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H44" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1502,22 +1798,25 @@
       <c r="A45" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>18</v>
+      <c r="B45" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G45" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H45" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1525,22 +1824,25 @@
       <c r="A46" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>96</v>
+      <c r="B46" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G46" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H46" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1548,22 +1850,25 @@
       <c r="A47" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>9</v>
+      <c r="B47" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G47" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H47" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1571,22 +1876,25 @@
       <c r="A48" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>21</v>
+      <c r="B48" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>111</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>21</v>
+        <v>111</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G48" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H48" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1594,22 +1902,25 @@
       <c r="A49" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>44</v>
+      <c r="B49" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G49" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H49" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1617,22 +1928,25 @@
       <c r="A50" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>21</v>
+      <c r="B50" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G50" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H50" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1640,26 +1954,30 @@
       <c r="A51" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>106</v>
+      <c r="B51" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>117</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G51" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H51" s="1" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H51"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1667,5 +1985,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Edit methods, results, discussion, conclusion, figures, abstract, and style, before submitting the second revision, #4
</commit_message>
<xml_diff>
--- a/law-firms-names/journal-article/cluster-labels.xlsx
+++ b/law-firms-names/journal-article/cluster-labels.xlsx
@@ -386,7 +386,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -420,11 +420,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -469,7 +464,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -488,10 +483,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -632,8 +623,8 @@
   </sheetPr>
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F43" activeCellId="0" sqref="F43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G43" activeCellId="0" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1368,7 +1359,7 @@
       <c r="E28" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="1" t="s">
         <v>70</v>
       </c>
       <c r="G28" s="1" t="s">
@@ -1762,7 +1753,7 @@
         <v>16</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="H43" s="1" t="n">
         <v>0</v>

</xml_diff>